<commit_message>
completed layout with internet connected module, updated gerbers and bom
</commit_message>
<xml_diff>
--- a/pcb/R1000AX_BOM.xlsx
+++ b/pcb/R1000AX_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="284">
   <si>
     <t>Reference</t>
   </si>
@@ -71,6 +71,9 @@
     <t>NXP Semiconductors</t>
   </si>
   <si>
+    <t>STUFF</t>
+  </si>
+  <si>
     <t>J25</t>
   </si>
   <si>
@@ -188,21 +191,6 @@
     <t>USB-B1HSW6</t>
   </si>
   <si>
-    <t>MP1</t>
-  </si>
-  <si>
-    <t>SDCARD_RECEPTACLE</t>
-  </si>
-  <si>
-    <t>Main:SDCARD_RECEPTACLE</t>
-  </si>
-  <si>
-    <t>Amphenol Commercial Products</t>
-  </si>
-  <si>
-    <t>101-00313-68-02</t>
-  </si>
-  <si>
     <t>J81</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>STUFF</t>
-  </si>
-  <si>
     <t>R67</t>
   </si>
   <si>
@@ -453,6 +438,12 @@
   </si>
   <si>
     <t>J18</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>J20</t>
   </si>
   <si>
     <t>J3</t>
@@ -949,12 +940,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -975,10 +962,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N120"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -989,14 +976,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3214285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.0255102040816"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.76530612244898"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.95408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.21428571428571"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.68367346938776"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.8469387755102"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.20408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.04591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.29081632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1060,196 +1047,208 @@
       <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>742792651</v>
       </c>
+      <c r="G5" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
+      <c r="G7" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>673298000</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>61</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,39 +1256,39 @@
         <v>62</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G14" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,559 +1299,571 @@
         <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>68</v>
       </c>
       <c r="G15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>71</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="K16" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>50</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="I24" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="I26" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="G28" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="K28" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G30" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="K33" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K33" s="0" t="s">
+      <c r="L33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M33" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,208 +1871,199 @@
         <v>111</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="K36" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M36" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="L36" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M36" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="I38" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="L38" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M38" s="0" t="s">
-        <v>115</v>
+        <v>71</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="F40" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,2016 +2071,2078 @@
         <v>127</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N41" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N42" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N43" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N44" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N45" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N45" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="E46" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="F46" s="0" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N46" s="0" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>142</v>
+        <v>59</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>142</v>
+        <v>61</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>150</v>
+        <v>52</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>673298000</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G50" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G51" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G52" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G53" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G54" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G55" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G56" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G57" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G58" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F59" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G59" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G60" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G61" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F62" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G62" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="G63" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>168</v>
+        <v>147</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>173</v>
+        <v>165</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E67" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F67" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="F67" s="0" t="s">
-        <v>181</v>
+      <c r="G67" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="L71" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="M71" s="0" t="s">
-        <v>197</v>
+        <v>71</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B72" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="K72" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="L72" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="E72" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="G72" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I72" s="0" t="s">
+      <c r="M72" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="K72" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="L72" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="M72" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="K73" s="0" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="L73" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M73" s="0" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K74" s="0" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="L74" s="0" t="s">
-        <v>104</v>
+        <v>193</v>
       </c>
       <c r="M74" s="0" t="s">
-        <v>83</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E75" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F75" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F75" s="0" t="s">
-        <v>204</v>
-      </c>
       <c r="G75" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>205</v>
+        <v>77</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M75" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>73</v>
+        <v>201</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>73</v>
+        <v>201</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="I76" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J76" s="0" t="s">
-        <v>77</v>
+      <c r="K76" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="L76" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M76" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K77" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="L77" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M77" s="0" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>209</v>
+        <v>74</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>193</v>
+        <v>75</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>210</v>
+        <v>69</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>209</v>
+        <v>74</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K78" s="0" t="s">
-        <v>201</v>
+        <v>77</v>
       </c>
       <c r="L78" s="0" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="M78" s="0" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>74</v>
+        <v>207</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I79" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="L79" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="M79" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="K79" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="L79" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="M79" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="K80" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="L80" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="E80" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I80" s="0" t="s">
+      <c r="M80" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="K80" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="L80" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="M80" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>189</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>189</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>190</v>
+        <v>24</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="J81" s="0" t="s">
-        <v>77</v>
+        <v>191</v>
+      </c>
+      <c r="K81" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="L81" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="M81" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>223</v>
+        <v>32</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>224</v>
+        <v>69</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>222</v>
+        <v>216</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>226</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B85" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="I85" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J85" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="E85" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="I85" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="J85" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J86" s="0" t="s">
-        <v>77</v>
+        <v>223</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>230</v>
+        <v>118</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>231</v>
+        <v>32</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>232</v>
+        <v>118</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J87" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>236</v>
+        <v>17</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>234</v>
+        <v>229</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>239</v>
+        <v>231</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>242</v>
+        <v>236</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>245</v>
+        <v>37</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>250</v>
+        <v>241</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>79</v>
+        <v>244</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>74</v>
+        <v>246</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>79</v>
+        <v>247</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I93" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K93" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="L93" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M93" s="0" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E94" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F94" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F94" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G94" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K94" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L94" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M94" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E95" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F95" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F95" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G95" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K95" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L95" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M95" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E96" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F96" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F96" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="G96" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K96" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L96" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M96" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E97" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F97" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F97" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="G97" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K97" s="0" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="L97" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M97" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H98" s="0" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="I98" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J98" s="0" t="s">
-        <v>77</v>
+      <c r="K98" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="L98" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M98" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H99" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H100" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H101" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H103" s="0" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H104" s="0" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H105" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>265</v>
+        <v>88</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>265</v>
+        <v>88</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H106" s="0" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H107" s="0" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H108" s="0" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H109" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H110" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H111" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H112" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I112" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J112" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H113" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I113" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>123</v>
+        <v>268</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F114" s="0" t="s">
-        <v>123</v>
+        <v>268</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H114" s="0" t="s">
-        <v>124</v>
+        <v>269</v>
       </c>
       <c r="I114" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H115" s="0" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="I115" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="F116" s="0" t="s">
-        <v>239</v>
+        <v>68</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H116" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J116" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>73</v>
+        <v>235</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="F118" s="0" t="s">
-        <v>73</v>
+        <v>236</v>
       </c>
       <c r="G118" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H118" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="I118" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="J118" s="0" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="H119" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="I119" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K119" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="L119" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M119" s="0" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="J119" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="F120" s="0" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
       <c r="G120" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N120" s="0" t="s">
-        <v>286</v>
+        <v>24</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K120" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="L120" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M120" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N121" s="0" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed v1.3.1, implemented changes based on second crowdsupply update
</commit_message>
<xml_diff>
--- a/pcb/R1000AX_BOM.xlsx
+++ b/pcb/R1000AX_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="217">
   <si>
     <t>Reference</t>
   </si>
@@ -173,6 +173,72 @@
     <t>12.0 pF</t>
   </si>
   <si>
+    <t>D1 </t>
+  </si>
+  <si>
+    <t>LTST-C171GKT</t>
+  </si>
+  <si>
+    <t>Main:DIOC200X120X110</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>STUFF</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>D2 </t>
+  </si>
+  <si>
+    <t>LTST-C171TBKT</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>D5 </t>
+  </si>
+  <si>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>Main:SOD3717X135</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>DLED1 DLED2 DLED3 DLED4 </t>
+  </si>
+  <si>
+    <t>LTW-170TK</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>DLED5 </t>
+  </si>
+  <si>
+    <t>LTST-C171KRKT</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>FID1 FID2 FID3 </t>
+  </si>
+  <si>
+    <t>FIDTOP001</t>
+  </si>
+  <si>
+    <t>Main:FIDTOP001</t>
+  </si>
+  <si>
     <t>J17 </t>
   </si>
   <si>
@@ -203,6 +269,21 @@
     <t>1586042-8</t>
   </si>
   <si>
+    <t>J1 J10 J11 J12 J13 J14 J15 J2 J3 J4 J5 J6 J7 J8 J9 </t>
+  </si>
+  <si>
+    <t>PCIESOCKET-X1</t>
+  </si>
+  <si>
+    <t>Main:PCIESOCKET-X1</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>10018784-10200TLF</t>
+  </si>
+  <si>
     <t>J20 J31 </t>
   </si>
   <si>
@@ -215,22 +296,31 @@
     <t>Molex, LLC</t>
   </si>
   <si>
-    <t>J81 J82 </t>
+    <t>J18 J83 </t>
   </si>
   <si>
     <t>SOCKET254P-01X02</t>
   </si>
   <si>
-    <t>Main:SOCKET254P-01X02</t>
+    <t>Main:SOCKET254P-01X02_2</t>
   </si>
   <si>
     <t>640456-2</t>
   </si>
   <si>
-    <t>J18 J83 </t>
-  </si>
-  <si>
-    <t>Main:SOCKET254P-01X02_2</t>
+    <t>L1 </t>
+  </si>
+  <si>
+    <t>INDUCTOR_SRN4026-2R2Y</t>
+  </si>
+  <si>
+    <t>Main:INDP400400X250</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>SRN4026-2R2Y</t>
   </si>
   <si>
     <t>L2 </t>
@@ -245,6 +335,78 @@
     <t>Wurth Electronics Inc</t>
   </si>
   <si>
+    <t>L3 </t>
+  </si>
+  <si>
+    <t>INDUCTOR_SRN6045TA-4R7M</t>
+  </si>
+  <si>
+    <t>Main:INDP600600X420</t>
+  </si>
+  <si>
+    <t>SRN6045TA-4R7M</t>
+  </si>
+  <si>
+    <t>MP3 </t>
+  </si>
+  <si>
+    <t>MICROSD_DM3AT-SF-PEJM5</t>
+  </si>
+  <si>
+    <t>Main:MICROSD_RECEPTACLE_2</t>
+  </si>
+  <si>
+    <t>Hirose Electric Co Ltd</t>
+  </si>
+  <si>
+    <t>DM3AT-SF-PEJM5</t>
+  </si>
+  <si>
+    <t>Q1 </t>
+  </si>
+  <si>
+    <t>DMG2305UX-7</t>
+  </si>
+  <si>
+    <t>Main:SOT190P290X130X100-3</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>Q2 </t>
+  </si>
+  <si>
+    <t>PSMN1R2-30YLC</t>
+  </si>
+  <si>
+    <t>Main:SOT127P500X110-5</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors</t>
+  </si>
+  <si>
+    <t>PSMN1R2-30YLC,115</t>
+  </si>
+  <si>
+    <t>Q3 Q5 Q6 </t>
+  </si>
+  <si>
+    <t>Q_PNP_BEC</t>
+  </si>
+  <si>
+    <t>MMBT4403LT3G</t>
+  </si>
+  <si>
+    <t>Q4 </t>
+  </si>
+  <si>
+    <t>Q_NPN_BEC</t>
+  </si>
+  <si>
+    <t>MMBT2222ALT3G</t>
+  </si>
+  <si>
     <t>R1 R2 R3 R4 R5 </t>
   </si>
   <si>
@@ -296,6 +458,21 @@
     <t>9.76 kΩ</t>
   </si>
   <si>
+    <t>R16 </t>
+  </si>
+  <si>
+    <t>RSENSE_WSL3637</t>
+  </si>
+  <si>
+    <t>Main:RESC940914X064</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>WSL36373L000FEA</t>
+  </si>
+  <si>
     <t>R24 </t>
   </si>
   <si>
@@ -393,180 +570,6 @@
   </si>
   <si>
     <t>6.04 kΩ</t>
-  </si>
-  <si>
-    <t>D1 </t>
-  </si>
-  <si>
-    <t>LTST-C171GKT</t>
-  </si>
-  <si>
-    <t>Main:DIOC200X120X110</t>
-  </si>
-  <si>
-    <t>Lite-On Inc.</t>
-  </si>
-  <si>
-    <t>STUFF</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>D2 </t>
-  </si>
-  <si>
-    <t>LTST-C171TBKT</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>D5 </t>
-  </si>
-  <si>
-    <t>MBR0520LT1G</t>
-  </si>
-  <si>
-    <t>Main:SOD3717X135</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>DLED1 DLED2 DLED3 DLED4 </t>
-  </si>
-  <si>
-    <t>LTW-170TK</t>
-  </si>
-  <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>DLED5 </t>
-  </si>
-  <si>
-    <t>LTST-C171KRKT</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>J1 J10 J11 J12 J13 J14 J15 J2 J3 J4 J5 J6 J7 J8 J9 </t>
-  </si>
-  <si>
-    <t>PCIESOCKET-X1</t>
-  </si>
-  <si>
-    <t>Main:PCIESOCKET-X1</t>
-  </si>
-  <si>
-    <t>Amphenol FCI</t>
-  </si>
-  <si>
-    <t>10018784-10200TLF</t>
-  </si>
-  <si>
-    <t>L1 </t>
-  </si>
-  <si>
-    <t>INDUCTOR_SRN4026-2R2Y</t>
-  </si>
-  <si>
-    <t>Main:INDP400400X250</t>
-  </si>
-  <si>
-    <t>Bourns Inc.</t>
-  </si>
-  <si>
-    <t>SRN4026-2R2Y</t>
-  </si>
-  <si>
-    <t>L3 </t>
-  </si>
-  <si>
-    <t>INDUCTOR_SRN6045TA-4R7M</t>
-  </si>
-  <si>
-    <t>Main:INDP600600X420</t>
-  </si>
-  <si>
-    <t>SRN6045TA-4R7M</t>
-  </si>
-  <si>
-    <t>MP3 </t>
-  </si>
-  <si>
-    <t>MICROSD_SCHD3A0100</t>
-  </si>
-  <si>
-    <t>Main:CONN_SCHD3A0100</t>
-  </si>
-  <si>
-    <t>ALPS</t>
-  </si>
-  <si>
-    <t>SCHD3A0100</t>
-  </si>
-  <si>
-    <t>Q1 </t>
-  </si>
-  <si>
-    <t>DMG2305UX-7</t>
-  </si>
-  <si>
-    <t>Main:SOT190P290X130X100-3</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>Q2 </t>
-  </si>
-  <si>
-    <t>PSMN1R2-30YLC</t>
-  </si>
-  <si>
-    <t>Main:SOT127P500X110-5</t>
-  </si>
-  <si>
-    <t>NXP Semiconductors</t>
-  </si>
-  <si>
-    <t>PSMN1R2-30YLC,115</t>
-  </si>
-  <si>
-    <t>Q3 Q5 Q6 </t>
-  </si>
-  <si>
-    <t>Q_PNP_BEC</t>
-  </si>
-  <si>
-    <t>MMBT4403LT3G</t>
-  </si>
-  <si>
-    <t>Q4 </t>
-  </si>
-  <si>
-    <t>Q_NPN_BEC</t>
-  </si>
-  <si>
-    <t>MMBT2222ALT3G</t>
-  </si>
-  <si>
-    <t>R16 </t>
-  </si>
-  <si>
-    <t>RSENSE_WSL3637</t>
-  </si>
-  <si>
-    <t>Main:RESC940914X064</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>WSL36373L000FEA</t>
   </si>
   <si>
     <t>S1 S2 S3 </t>
@@ -761,12 +764,12 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N49" activeCellId="0" sqref="N49"/>
+      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9183673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8520408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.219387755102"/>
@@ -1128,189 +1131,174 @@
         <v>55</v>
       </c>
       <c r="G10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>19</v>
+      <c r="O10" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="H11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>673298000</v>
+      <c r="G12" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>742792651</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="G17" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,933 +1306,939 @@
         <v>84</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>673298000</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>742792651</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="G23" s="0" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="F28" s="0" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="O31" s="0" t="s">
-        <v>131</v>
+        <v>19</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="O32" s="0" t="s">
+      <c r="K32" s="0" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="O34" s="0" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="O35" s="0" t="s">
-        <v>144</v>
+        <v>19</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>148</v>
+        <v>18</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>153</v>
+        <v>18</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>171</v>
+        <v>18</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>182</v>
+        <v>18</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>183</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D46" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="F46" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>190</v>
-      </c>
       <c r="H46" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G48" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="F48" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="H48" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G49" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="F49" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>201</v>
-      </c>
       <c r="H49" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D50" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="G50" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="F50" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>205</v>
-      </c>
       <c r="H50" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="D51" s="0" t="s">
+      <c r="G51" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="F51" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="H51" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added host USB to LPC USB jump option using a diffpair
</commit_message>
<xml_diff>
--- a/pcb/R1000AX_BOM.xlsx
+++ b/pcb/R1000AX_BOM.xlsx
@@ -758,26 +758,26 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.95408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.15816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.68367346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.20408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.83673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.2448979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.83673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.87244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.71428571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.04591836734694"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -2223,11 +2223,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ready for 1.3.2 crowdsupply release
</commit_message>
<xml_diff>
--- a/pcb/R1000AX_BOM.xlsx
+++ b/pcb/R1000AX_BOM.xlsx
@@ -764,12 +764,12 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9183673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8520408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.219387755102"/>

</xml_diff>